<commit_message>
Preenchimento Diario de Bordo
</commit_message>
<xml_diff>
--- a/Documentação/diario_de_bordo/Diario de Bordo.xlsx
+++ b/Documentação/diario_de_bordo/Diario de Bordo.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Pi2\pi-segundo-semestre-2025\documentação\diario_de_bordo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\pi-2\pi-segundo-semestre-2025\Documentação\diario_de_bordo\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D31520A-8B5C-494D-8BDF-32452E5677D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Diário de Bordo" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
   <si>
     <t>DIARIO DE BORDO - NEXBIT</t>
   </si>
@@ -138,13 +139,16 @@
   </si>
   <si>
     <t>Organizando as pastas de documentação e diario de bordo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Correção/modificação do backend de login </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -181,8 +185,15 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -234,6 +245,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -318,7 +335,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -404,6 +421,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -744,31 +764,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="G3:S99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D69" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="N82" sqref="N82:O82"/>
+    <sheetView tabSelected="1" topLeftCell="H58" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="R84" sqref="R84"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="14.58203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="14.4140625" customWidth="1"/>
-    <col min="9" max="9" width="14.1640625" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
-    <col min="11" max="11" width="16.1640625" customWidth="1"/>
-    <col min="12" max="12" width="14.25" customWidth="1"/>
+    <col min="11" max="11" width="16.140625" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" customWidth="1"/>
     <col min="13" max="13" width="17" customWidth="1"/>
-    <col min="14" max="14" width="12.83203125" customWidth="1"/>
-    <col min="15" max="15" width="13.25" customWidth="1"/>
-    <col min="16" max="16" width="57.75" style="7" customWidth="1"/>
-    <col min="17" max="17" width="52.25" customWidth="1"/>
-    <col min="18" max="18" width="42.83203125" customWidth="1"/>
-    <col min="19" max="19" width="41.4140625" customWidth="1"/>
+    <col min="14" max="14" width="12.85546875" customWidth="1"/>
+    <col min="15" max="15" width="13.28515625" customWidth="1"/>
+    <col min="16" max="16" width="57.7109375" style="7" customWidth="1"/>
+    <col min="17" max="17" width="52.28515625" customWidth="1"/>
+    <col min="18" max="18" width="42.85546875" customWidth="1"/>
+    <col min="19" max="19" width="41.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="7:19" ht="15" customHeight="1">
+    <row r="3" spans="7:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G3" s="25" t="s">
         <v>0</v>
       </c>
@@ -785,7 +805,7 @@
       <c r="R3" s="26"/>
       <c r="S3" s="26"/>
     </row>
-    <row r="4" spans="7:19" ht="15" customHeight="1">
+    <row r="4" spans="7:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G4" s="27"/>
       <c r="H4" s="28"/>
       <c r="I4" s="28"/>
@@ -800,7 +820,7 @@
       <c r="R4" s="28"/>
       <c r="S4" s="28"/>
     </row>
-    <row r="5" spans="7:19">
+    <row r="5" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G5" s="29" t="s">
         <v>6</v>
       </c>
@@ -833,7 +853,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="7:19" ht="13.75" customHeight="1">
+    <row r="6" spans="7:19" ht="13.7" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G6" s="29"/>
       <c r="H6" s="30"/>
       <c r="I6" s="30"/>
@@ -848,7 +868,7 @@
       <c r="R6" s="23"/>
       <c r="S6" s="24"/>
     </row>
-    <row r="7" spans="7:19">
+    <row r="7" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G7" s="2">
         <v>45901</v>
       </c>
@@ -865,7 +885,7 @@
       <c r="R7" s="5"/>
       <c r="S7" s="5"/>
     </row>
-    <row r="8" spans="7:19">
+    <row r="8" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G8" s="2">
         <v>45902</v>
       </c>
@@ -882,7 +902,7 @@
       <c r="R8" s="5"/>
       <c r="S8" s="5"/>
     </row>
-    <row r="9" spans="7:19">
+    <row r="9" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G9" s="2">
         <v>45903</v>
       </c>
@@ -899,7 +919,7 @@
       <c r="R9" s="5"/>
       <c r="S9" s="5"/>
     </row>
-    <row r="10" spans="7:19">
+    <row r="10" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G10" s="2">
         <v>45904</v>
       </c>
@@ -916,7 +936,7 @@
       <c r="R10" s="5"/>
       <c r="S10" s="5"/>
     </row>
-    <row r="11" spans="7:19">
+    <row r="11" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G11" s="2">
         <v>45905</v>
       </c>
@@ -933,7 +953,7 @@
       <c r="R11" s="5"/>
       <c r="S11" s="5"/>
     </row>
-    <row r="12" spans="7:19">
+    <row r="12" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G12" s="2">
         <v>45906</v>
       </c>
@@ -950,7 +970,7 @@
       <c r="R12" s="5"/>
       <c r="S12" s="5"/>
     </row>
-    <row r="13" spans="7:19">
+    <row r="13" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G13" s="2">
         <v>45907</v>
       </c>
@@ -967,7 +987,7 @@
       <c r="R13" s="5"/>
       <c r="S13" s="5"/>
     </row>
-    <row r="14" spans="7:19">
+    <row r="14" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G14" s="2">
         <v>45908</v>
       </c>
@@ -984,7 +1004,7 @@
       <c r="R14" s="5"/>
       <c r="S14" s="5"/>
     </row>
-    <row r="15" spans="7:19">
+    <row r="15" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G15" s="2">
         <v>45909</v>
       </c>
@@ -1001,7 +1021,7 @@
       <c r="R15" s="5"/>
       <c r="S15" s="5"/>
     </row>
-    <row r="16" spans="7:19">
+    <row r="16" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G16" s="2">
         <v>45910</v>
       </c>
@@ -1028,7 +1048,7 @@
       <c r="R16" s="5"/>
       <c r="S16" s="5"/>
     </row>
-    <row r="17" spans="7:19">
+    <row r="17" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G17" s="2">
         <v>45911</v>
       </c>
@@ -1051,7 +1071,7 @@
       <c r="R17" s="5"/>
       <c r="S17" s="5"/>
     </row>
-    <row r="18" spans="7:19">
+    <row r="18" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G18" s="2">
         <v>45912</v>
       </c>
@@ -1068,7 +1088,7 @@
       <c r="R18" s="5"/>
       <c r="S18" s="5"/>
     </row>
-    <row r="19" spans="7:19">
+    <row r="19" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G19" s="2">
         <v>45913</v>
       </c>
@@ -1085,7 +1105,7 @@
       <c r="R19" s="5"/>
       <c r="S19" s="5"/>
     </row>
-    <row r="20" spans="7:19">
+    <row r="20" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G20" s="2">
         <v>45914</v>
       </c>
@@ -1106,7 +1126,7 @@
       <c r="R20" s="5"/>
       <c r="S20" s="5"/>
     </row>
-    <row r="21" spans="7:19">
+    <row r="21" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G21" s="2">
         <v>45915</v>
       </c>
@@ -1123,7 +1143,7 @@
       <c r="R21" s="5"/>
       <c r="S21" s="5"/>
     </row>
-    <row r="22" spans="7:19" ht="42">
+    <row r="22" spans="7:19" ht="45" x14ac:dyDescent="0.25">
       <c r="G22" s="2">
         <v>45916</v>
       </c>
@@ -1152,7 +1172,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="7:19">
+    <row r="23" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G23" s="2">
         <v>45917</v>
       </c>
@@ -1169,7 +1189,7 @@
       <c r="R23" s="5"/>
       <c r="S23" s="5"/>
     </row>
-    <row r="24" spans="7:19">
+    <row r="24" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G24" s="2">
         <v>45918</v>
       </c>
@@ -1186,7 +1206,7 @@
       <c r="R24" s="5"/>
       <c r="S24" s="5"/>
     </row>
-    <row r="25" spans="7:19">
+    <row r="25" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G25" s="2">
         <v>45919</v>
       </c>
@@ -1203,7 +1223,7 @@
       <c r="R25" s="5"/>
       <c r="S25" s="5"/>
     </row>
-    <row r="26" spans="7:19">
+    <row r="26" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G26" s="2">
         <v>45920</v>
       </c>
@@ -1220,7 +1240,7 @@
       <c r="R26" s="5"/>
       <c r="S26" s="5"/>
     </row>
-    <row r="27" spans="7:19">
+    <row r="27" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G27" s="2">
         <v>45921</v>
       </c>
@@ -1237,7 +1257,7 @@
       <c r="R27" s="5"/>
       <c r="S27" s="5"/>
     </row>
-    <row r="28" spans="7:19">
+    <row r="28" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G28" s="2">
         <v>45922</v>
       </c>
@@ -1254,7 +1274,7 @@
       <c r="R28" s="5"/>
       <c r="S28" s="5"/>
     </row>
-    <row r="29" spans="7:19">
+    <row r="29" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G29" s="2">
         <v>45923</v>
       </c>
@@ -1271,7 +1291,7 @@
       <c r="R29" s="5"/>
       <c r="S29" s="5"/>
     </row>
-    <row r="30" spans="7:19">
+    <row r="30" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G30" s="2">
         <v>45924</v>
       </c>
@@ -1288,7 +1308,7 @@
       <c r="R30" s="5"/>
       <c r="S30" s="5"/>
     </row>
-    <row r="31" spans="7:19" ht="28">
+    <row r="31" spans="7:19" ht="30" x14ac:dyDescent="0.25">
       <c r="G31" s="2">
         <v>45925</v>
       </c>
@@ -1311,7 +1331,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="32" spans="7:19">
+    <row r="32" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G32" s="2">
         <v>45926</v>
       </c>
@@ -1328,7 +1348,7 @@
       <c r="R32" s="5"/>
       <c r="S32" s="5"/>
     </row>
-    <row r="33" spans="7:19">
+    <row r="33" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G33" s="2">
         <v>45927</v>
       </c>
@@ -1345,7 +1365,7 @@
       <c r="R33" s="5"/>
       <c r="S33" s="5"/>
     </row>
-    <row r="34" spans="7:19">
+    <row r="34" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G34" s="2">
         <v>45928</v>
       </c>
@@ -1368,7 +1388,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="35" spans="7:19">
+    <row r="35" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G35" s="2">
         <v>45929</v>
       </c>
@@ -1389,7 +1409,7 @@
       <c r="R35" s="5"/>
       <c r="S35" s="5"/>
     </row>
-    <row r="36" spans="7:19" ht="28">
+    <row r="36" spans="7:19" ht="30" x14ac:dyDescent="0.25">
       <c r="G36" s="2">
         <v>45930</v>
       </c>
@@ -1410,7 +1430,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="7:19">
+    <row r="37" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G37" s="2">
         <v>45931</v>
       </c>
@@ -1427,7 +1447,7 @@
       <c r="R37" s="5"/>
       <c r="S37" s="5"/>
     </row>
-    <row r="38" spans="7:19" ht="28">
+    <row r="38" spans="7:19" ht="30" x14ac:dyDescent="0.25">
       <c r="G38" s="2">
         <v>45932</v>
       </c>
@@ -1450,7 +1470,7 @@
       <c r="R38" s="5"/>
       <c r="S38" s="5"/>
     </row>
-    <row r="39" spans="7:19">
+    <row r="39" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G39" s="2">
         <v>45933</v>
       </c>
@@ -1477,7 +1497,7 @@
       <c r="R39" s="5"/>
       <c r="S39" s="5"/>
     </row>
-    <row r="40" spans="7:19" ht="28">
+    <row r="40" spans="7:19" ht="30" x14ac:dyDescent="0.25">
       <c r="G40" s="2">
         <v>45934</v>
       </c>
@@ -1498,7 +1518,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="7:19">
+    <row r="41" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G41" s="2">
         <v>45935</v>
       </c>
@@ -1519,7 +1539,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="42" spans="7:19">
+    <row r="42" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G42" s="2">
         <v>45936</v>
       </c>
@@ -1536,7 +1556,7 @@
       <c r="R42" s="5"/>
       <c r="S42" s="5"/>
     </row>
-    <row r="43" spans="7:19">
+    <row r="43" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G43" s="2">
         <v>45937</v>
       </c>
@@ -1553,7 +1573,7 @@
       <c r="R43" s="5"/>
       <c r="S43" s="5"/>
     </row>
-    <row r="44" spans="7:19">
+    <row r="44" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G44" s="2">
         <v>45938</v>
       </c>
@@ -1570,7 +1590,7 @@
       <c r="R44" s="5"/>
       <c r="S44" s="5"/>
     </row>
-    <row r="45" spans="7:19">
+    <row r="45" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G45" s="2">
         <v>45939</v>
       </c>
@@ -1591,7 +1611,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="46" spans="7:19" ht="28">
+    <row r="46" spans="7:19" ht="30" x14ac:dyDescent="0.25">
       <c r="G46" s="2">
         <v>45940</v>
       </c>
@@ -1616,7 +1636,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="47" spans="7:19">
+    <row r="47" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G47" s="2">
         <v>45941</v>
       </c>
@@ -1633,7 +1653,7 @@
       <c r="R47" s="5"/>
       <c r="S47" s="5"/>
     </row>
-    <row r="48" spans="7:19">
+    <row r="48" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G48" s="2">
         <v>45942</v>
       </c>
@@ -1650,7 +1670,7 @@
       <c r="R48" s="5"/>
       <c r="S48" s="5"/>
     </row>
-    <row r="49" spans="7:19">
+    <row r="49" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G49" s="2">
         <v>45943</v>
       </c>
@@ -1667,7 +1687,7 @@
       <c r="R49" s="5"/>
       <c r="S49" s="5"/>
     </row>
-    <row r="50" spans="7:19">
+    <row r="50" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G50" s="2">
         <v>45944</v>
       </c>
@@ -1690,7 +1710,7 @@
       <c r="R50" s="5"/>
       <c r="S50" s="5"/>
     </row>
-    <row r="51" spans="7:19">
+    <row r="51" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G51" s="2">
         <v>45945</v>
       </c>
@@ -1713,7 +1733,7 @@
       <c r="R51" s="5"/>
       <c r="S51" s="5"/>
     </row>
-    <row r="52" spans="7:19">
+    <row r="52" spans="7:19" ht="30" x14ac:dyDescent="0.25">
       <c r="G52" s="2">
         <v>45946</v>
       </c>
@@ -1736,7 +1756,7 @@
       <c r="R52" s="5"/>
       <c r="S52" s="5"/>
     </row>
-    <row r="53" spans="7:19" ht="56">
+    <row r="53" spans="7:19" ht="60" x14ac:dyDescent="0.25">
       <c r="G53" s="2">
         <v>45947</v>
       </c>
@@ -1759,7 +1779,7 @@
       <c r="R53" s="5"/>
       <c r="S53" s="5"/>
     </row>
-    <row r="54" spans="7:19" ht="28">
+    <row r="54" spans="7:19" ht="45" x14ac:dyDescent="0.25">
       <c r="G54" s="2">
         <v>45948</v>
       </c>
@@ -1782,7 +1802,7 @@
       <c r="R54" s="5"/>
       <c r="S54" s="5"/>
     </row>
-    <row r="55" spans="7:19">
+    <row r="55" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G55" s="2">
         <v>45949</v>
       </c>
@@ -1799,7 +1819,7 @@
       <c r="R55" s="5"/>
       <c r="S55" s="5"/>
     </row>
-    <row r="56" spans="7:19">
+    <row r="56" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G56" s="2">
         <v>45950</v>
       </c>
@@ -1816,7 +1836,7 @@
       <c r="R56" s="5"/>
       <c r="S56" s="5"/>
     </row>
-    <row r="57" spans="7:19" ht="28">
+    <row r="57" spans="7:19" ht="30" x14ac:dyDescent="0.25">
       <c r="G57" s="2">
         <v>45951</v>
       </c>
@@ -1839,7 +1859,7 @@
       <c r="R57" s="5"/>
       <c r="S57" s="5"/>
     </row>
-    <row r="58" spans="7:19">
+    <row r="58" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G58" s="2">
         <v>45952</v>
       </c>
@@ -1856,7 +1876,7 @@
       <c r="R58" s="5"/>
       <c r="S58" s="5"/>
     </row>
-    <row r="59" spans="7:19" ht="28">
+    <row r="59" spans="7:19" ht="45" x14ac:dyDescent="0.25">
       <c r="G59" s="2">
         <v>45953</v>
       </c>
@@ -1879,7 +1899,7 @@
       <c r="R59" s="5"/>
       <c r="S59" s="5"/>
     </row>
-    <row r="60" spans="7:19">
+    <row r="60" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G60" s="2">
         <v>45954</v>
       </c>
@@ -1902,7 +1922,7 @@
       <c r="R60" s="5"/>
       <c r="S60" s="5"/>
     </row>
-    <row r="61" spans="7:19">
+    <row r="61" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G61" s="2">
         <v>45955</v>
       </c>
@@ -1919,7 +1939,7 @@
       <c r="R61" s="5"/>
       <c r="S61" s="5"/>
     </row>
-    <row r="62" spans="7:19">
+    <row r="62" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G62" s="2">
         <v>45956</v>
       </c>
@@ -1936,7 +1956,7 @@
       <c r="R62" s="5"/>
       <c r="S62" s="5"/>
     </row>
-    <row r="63" spans="7:19">
+    <row r="63" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G63" s="2">
         <v>45957</v>
       </c>
@@ -1953,7 +1973,7 @@
       <c r="R63" s="5"/>
       <c r="S63" s="5"/>
     </row>
-    <row r="64" spans="7:19">
+    <row r="64" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G64" s="2">
         <v>45958</v>
       </c>
@@ -1970,7 +1990,7 @@
       <c r="R64" s="5"/>
       <c r="S64" s="5"/>
     </row>
-    <row r="65" spans="7:19" ht="28">
+    <row r="65" spans="7:19" ht="30" x14ac:dyDescent="0.25">
       <c r="G65" s="2">
         <v>45959</v>
       </c>
@@ -1993,7 +2013,7 @@
       <c r="R65" s="5"/>
       <c r="S65" s="5"/>
     </row>
-    <row r="66" spans="7:19">
+    <row r="66" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G66" s="2">
         <v>45960</v>
       </c>
@@ -2010,7 +2030,7 @@
       <c r="R66" s="5"/>
       <c r="S66" s="5"/>
     </row>
-    <row r="67" spans="7:19">
+    <row r="67" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G67" s="19">
         <v>45961</v>
       </c>
@@ -2033,7 +2053,7 @@
       <c r="R67" s="20"/>
       <c r="S67" s="20"/>
     </row>
-    <row r="68" spans="7:19">
+    <row r="68" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G68" s="19">
         <v>45962</v>
       </c>
@@ -2050,7 +2070,7 @@
       <c r="R68" s="20"/>
       <c r="S68" s="20"/>
     </row>
-    <row r="69" spans="7:19">
+    <row r="69" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G69" s="19">
         <v>45963</v>
       </c>
@@ -2067,7 +2087,7 @@
       <c r="R69" s="20"/>
       <c r="S69" s="20"/>
     </row>
-    <row r="70" spans="7:19">
+    <row r="70" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G70" s="19">
         <v>45964</v>
       </c>
@@ -2084,7 +2104,7 @@
       <c r="R70" s="20"/>
       <c r="S70" s="20"/>
     </row>
-    <row r="71" spans="7:19">
+    <row r="71" spans="7:19" ht="30" x14ac:dyDescent="0.25">
       <c r="G71" s="19">
         <v>45965</v>
       </c>
@@ -2105,7 +2125,7 @@
       </c>
       <c r="S71" s="20"/>
     </row>
-    <row r="72" spans="7:19" ht="28">
+    <row r="72" spans="7:19" ht="30" x14ac:dyDescent="0.25">
       <c r="G72" s="19">
         <v>45966</v>
       </c>
@@ -2126,7 +2146,7 @@
       </c>
       <c r="S72" s="20"/>
     </row>
-    <row r="73" spans="7:19">
+    <row r="73" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G73" s="19">
         <v>45967</v>
       </c>
@@ -2143,7 +2163,7 @@
       <c r="R73" s="20"/>
       <c r="S73" s="20"/>
     </row>
-    <row r="74" spans="7:19">
+    <row r="74" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G74" s="19">
         <v>45968</v>
       </c>
@@ -2160,7 +2180,7 @@
       <c r="R74" s="20"/>
       <c r="S74" s="20"/>
     </row>
-    <row r="75" spans="7:19">
+    <row r="75" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G75" s="19">
         <v>45969</v>
       </c>
@@ -2177,7 +2197,7 @@
       <c r="R75" s="20"/>
       <c r="S75" s="20"/>
     </row>
-    <row r="76" spans="7:19">
+    <row r="76" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G76" s="19">
         <v>45970</v>
       </c>
@@ -2194,7 +2214,7 @@
       <c r="R76" s="20"/>
       <c r="S76" s="20"/>
     </row>
-    <row r="77" spans="7:19">
+    <row r="77" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G77" s="19">
         <v>45971</v>
       </c>
@@ -2211,7 +2231,7 @@
       <c r="R77" s="20"/>
       <c r="S77" s="20"/>
     </row>
-    <row r="78" spans="7:19">
+    <row r="78" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G78" s="19">
         <v>45972</v>
       </c>
@@ -2228,7 +2248,7 @@
       <c r="R78" s="20"/>
       <c r="S78" s="20"/>
     </row>
-    <row r="79" spans="7:19">
+    <row r="79" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G79" s="19">
         <v>45973</v>
       </c>
@@ -2245,7 +2265,7 @@
       <c r="R79" s="20"/>
       <c r="S79" s="20"/>
     </row>
-    <row r="80" spans="7:19">
+    <row r="80" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G80" s="19">
         <v>45974</v>
       </c>
@@ -2262,7 +2282,7 @@
       <c r="R80" s="20"/>
       <c r="S80" s="20"/>
     </row>
-    <row r="81" spans="7:19">
+    <row r="81" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G81" s="19">
         <v>45975</v>
       </c>
@@ -2279,7 +2299,7 @@
       <c r="R81" s="20"/>
       <c r="S81" s="20"/>
     </row>
-    <row r="82" spans="7:19" ht="28">
+    <row r="82" spans="7:19" ht="30" x14ac:dyDescent="0.25">
       <c r="G82" s="19">
         <v>45976</v>
       </c>
@@ -2302,7 +2322,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="83" spans="7:19">
+    <row r="83" spans="7:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="G83" s="19">
         <v>45977</v>
       </c>
@@ -2311,15 +2331,19 @@
       <c r="J83" s="20"/>
       <c r="K83" s="20"/>
       <c r="L83" s="20"/>
-      <c r="M83" s="20"/>
+      <c r="M83" s="31">
+        <v>45977</v>
+      </c>
       <c r="N83" s="20"/>
       <c r="O83" s="20"/>
       <c r="P83" s="18"/>
       <c r="Q83" s="20"/>
-      <c r="R83" s="20"/>
+      <c r="R83" s="16" t="s">
+        <v>38</v>
+      </c>
       <c r="S83" s="20"/>
     </row>
-    <row r="84" spans="7:19">
+    <row r="84" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G84" s="19">
         <v>45978</v>
       </c>
@@ -2336,7 +2360,7 @@
       <c r="R84" s="20"/>
       <c r="S84" s="20"/>
     </row>
-    <row r="85" spans="7:19">
+    <row r="85" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G85" s="19">
         <v>45979</v>
       </c>
@@ -2353,7 +2377,7 @@
       <c r="R85" s="20"/>
       <c r="S85" s="20"/>
     </row>
-    <row r="86" spans="7:19">
+    <row r="86" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G86" s="19">
         <v>45980</v>
       </c>
@@ -2370,7 +2394,7 @@
       <c r="R86" s="20"/>
       <c r="S86" s="20"/>
     </row>
-    <row r="87" spans="7:19">
+    <row r="87" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G87" s="19">
         <v>45981</v>
       </c>
@@ -2387,7 +2411,7 @@
       <c r="R87" s="20"/>
       <c r="S87" s="20"/>
     </row>
-    <row r="88" spans="7:19">
+    <row r="88" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G88" s="19">
         <v>45982</v>
       </c>
@@ -2404,7 +2428,7 @@
       <c r="R88" s="20"/>
       <c r="S88" s="20"/>
     </row>
-    <row r="89" spans="7:19">
+    <row r="89" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G89" s="19">
         <v>45983</v>
       </c>
@@ -2421,7 +2445,7 @@
       <c r="R89" s="20"/>
       <c r="S89" s="20"/>
     </row>
-    <row r="90" spans="7:19">
+    <row r="90" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G90" s="19">
         <v>45984</v>
       </c>
@@ -2438,7 +2462,7 @@
       <c r="R90" s="20"/>
       <c r="S90" s="20"/>
     </row>
-    <row r="91" spans="7:19">
+    <row r="91" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G91" s="19">
         <v>45985</v>
       </c>
@@ -2455,7 +2479,7 @@
       <c r="R91" s="20"/>
       <c r="S91" s="20"/>
     </row>
-    <row r="92" spans="7:19">
+    <row r="92" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G92" s="19">
         <v>45986</v>
       </c>
@@ -2472,7 +2496,7 @@
       <c r="R92" s="20"/>
       <c r="S92" s="20"/>
     </row>
-    <row r="93" spans="7:19">
+    <row r="93" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G93" s="19">
         <v>45987</v>
       </c>
@@ -2489,7 +2513,7 @@
       <c r="R93" s="20"/>
       <c r="S93" s="20"/>
     </row>
-    <row r="94" spans="7:19">
+    <row r="94" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G94" s="19">
         <v>45988</v>
       </c>
@@ -2506,7 +2530,7 @@
       <c r="R94" s="20"/>
       <c r="S94" s="20"/>
     </row>
-    <row r="95" spans="7:19">
+    <row r="95" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G95" s="19">
         <v>45989</v>
       </c>
@@ -2523,7 +2547,7 @@
       <c r="R95" s="20"/>
       <c r="S95" s="20"/>
     </row>
-    <row r="96" spans="7:19">
+    <row r="96" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G96" s="19">
         <v>45990</v>
       </c>
@@ -2540,7 +2564,7 @@
       <c r="R96" s="20"/>
       <c r="S96" s="20"/>
     </row>
-    <row r="97" spans="7:19">
+    <row r="97" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G97" s="19">
         <v>45991</v>
       </c>
@@ -2557,7 +2581,7 @@
       <c r="R97" s="20"/>
       <c r="S97" s="20"/>
     </row>
-    <row r="98" spans="7:19">
+    <row r="98" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G98" s="19">
         <v>45992</v>
       </c>
@@ -2574,7 +2598,7 @@
       <c r="R98" s="20"/>
       <c r="S98" s="20"/>
     </row>
-    <row r="99" spans="7:19">
+    <row r="99" spans="7:19" x14ac:dyDescent="0.25">
       <c r="G99" s="19">
         <v>45993</v>
       </c>

</xml_diff>